<commit_message>
Sauvegarde du projet "v2 - 2013"
</commit_message>
<xml_diff>
--- a/Info/StrategyGenerator/v2 - 2013/Conception/Ratio.xlsx
+++ b/Info/StrategyGenerator/v2 - 2013/Conception/Ratio.xlsx
@@ -377,6 +377,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -384,15 +393,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -699,7 +699,7 @@
   <dimension ref="A1:I16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I13" sqref="I13"/>
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -718,21 +718,21 @@
     </row>
     <row r="2" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="13" t="s">
+      <c r="A3" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="14"/>
-      <c r="C3" s="15"/>
-      <c r="D3" s="16" t="s">
+      <c r="B3" s="17"/>
+      <c r="C3" s="18"/>
+      <c r="D3" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="E3" s="17"/>
-      <c r="F3" s="18"/>
-      <c r="G3" s="16" t="s">
+      <c r="E3" s="14"/>
+      <c r="F3" s="15"/>
+      <c r="G3" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="H3" s="17"/>
-      <c r="I3" s="18"/>
+      <c r="H3" s="14"/>
+      <c r="I3" s="15"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="10"/>
@@ -785,7 +785,7 @@
         <v>295</v>
       </c>
       <c r="I5" s="6">
-        <f>$B$1*H5</f>
+        <f t="shared" ref="I5:I13" si="0">$B$1*H5</f>
         <v>59</v>
       </c>
     </row>
@@ -817,7 +817,7 @@
         <v>450</v>
       </c>
       <c r="I6" s="6">
-        <f>$B$1*H6</f>
+        <f t="shared" si="0"/>
         <v>90</v>
       </c>
     </row>
@@ -840,7 +840,7 @@
         <v>22.692307692307693</v>
       </c>
       <c r="I7" s="6">
-        <f>$B$1*H7</f>
+        <f t="shared" si="0"/>
         <v>4.5384615384615392</v>
       </c>
     </row>
@@ -855,13 +855,13 @@
         <v>45</v>
       </c>
       <c r="F8" s="6">
-        <f>$B$1*E8</f>
+        <f t="shared" ref="F8:F13" si="1">$B$1*E8</f>
         <v>9</v>
       </c>
       <c r="G8" s="5"/>
       <c r="H8" s="2"/>
       <c r="I8" s="6">
-        <f>$B$1*H8</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -876,13 +876,13 @@
         <v>35</v>
       </c>
       <c r="F9" s="6">
-        <f>$B$1*E9</f>
+        <f t="shared" si="1"/>
         <v>7</v>
       </c>
       <c r="G9" s="5"/>
       <c r="H9" s="2"/>
       <c r="I9" s="6">
-        <f>$B$1*H9</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -897,13 +897,13 @@
         <v>135</v>
       </c>
       <c r="F10" s="6">
-        <f>$B$1*E10</f>
+        <f t="shared" si="1"/>
         <v>27</v>
       </c>
       <c r="G10" s="5"/>
       <c r="H10" s="2"/>
       <c r="I10" s="6">
-        <f>$B$1*H10</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -914,13 +914,13 @@
       <c r="D11" s="5"/>
       <c r="E11" s="2"/>
       <c r="F11" s="6">
-        <f>$B$1*E11</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="G11" s="5"/>
       <c r="H11" s="2"/>
       <c r="I11" s="6">
-        <f>$B$1*H11</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -931,13 +931,13 @@
       <c r="D12" s="5"/>
       <c r="E12" s="2"/>
       <c r="F12" s="6">
-        <f>$B$1*E12</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="G12" s="5"/>
       <c r="H12" s="2"/>
       <c r="I12" s="6">
-        <f>$B$1*H12</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -948,13 +948,13 @@
       <c r="D13" s="5"/>
       <c r="E13" s="2"/>
       <c r="F13" s="6">
-        <f>$B$1*E13</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="G13" s="5"/>
       <c r="H13" s="2"/>
       <c r="I13" s="6">
-        <f>$B$1*H13</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>

</xml_diff>